<commit_message>
correct Anne-Laure P name
</commit_message>
<xml_diff>
--- a/data/matchs.xlsx
+++ b/data/matchs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="40">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">Maximilien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anne-LaureP</t>
   </si>
   <si>
     <t xml:space="preserve">Anna</t>
@@ -432,8 +429,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A147" activeCellId="0" sqref="A147:A149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E72" activeCellId="0" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="24" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -442,7 +439,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="10.84"/>
   </cols>
@@ -1881,7 +1878,7 @@
         <v>27</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>11</v>
@@ -2755,7 +2752,7 @@
         <v>20</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D116" s="11" t="s">
         <v>13</v>
@@ -2818,7 +2815,7 @@
         <v>13</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E119" s="11" t="s">
         <v>18</v>
@@ -3021,7 +3018,7 @@
         <v>18</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F129" s="11" t="s">
         <v>10</v>
@@ -3061,7 +3058,7 @@
         <v>18</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>11</v>
@@ -3138,7 +3135,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E135" s="11" t="s">
         <v>18</v>

</xml_diff>